<commit_message>
new ways to get survivors
</commit_message>
<xml_diff>
--- a/data/info.xlsx
+++ b/data/info.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D96B2CA-838F-4A83-8720-29AE62FF98AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A55C927-D17D-4757-9564-1461178457E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map_tiles" sheetId="2" r:id="rId1"/>
@@ -2357,8 +2357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EDFAF7-3A54-4002-A96B-C2CBDBF3D89B}">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3872,7 +3872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE295004-92D0-4869-98E3-E69FBF91F6CE}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -3906,7 +3906,7 @@
         <v>106</v>
       </c>
       <c r="D2" s="33">
-        <f>B2/SUM(B:B)</f>
+        <f t="shared" ref="D2:D23" si="0">B2/SUM(B:B)</f>
         <v>6.4220183486238536E-2</v>
       </c>
       <c r="E2" t="str">
@@ -3925,7 +3925,7 @@
         <v>106</v>
       </c>
       <c r="D3" s="33">
-        <f>B3/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>6.4220183486238536E-2</v>
       </c>
       <c r="E3" t="str">
@@ -3944,7 +3944,7 @@
         <v>106</v>
       </c>
       <c r="D4" s="33">
-        <f>B4/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>6.4220183486238536E-2</v>
       </c>
       <c r="E4" t="str">
@@ -3963,7 +3963,7 @@
         <v>106</v>
       </c>
       <c r="D5" s="33">
-        <f>B5/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>6.4220183486238536E-2</v>
       </c>
       <c r="E5" t="str">
@@ -3982,7 +3982,7 @@
         <v>106</v>
       </c>
       <c r="D6" s="33">
-        <f>B6/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>6.4220183486238536E-2</v>
       </c>
       <c r="E6" t="str">
@@ -4001,7 +4001,7 @@
         <v>106</v>
       </c>
       <c r="D7" s="33">
-        <f>B7/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>6.4220183486238536E-2</v>
       </c>
       <c r="E7" t="str">
@@ -4020,7 +4020,7 @@
         <v>106</v>
       </c>
       <c r="D8" s="33">
-        <f>B8/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>6.4220183486238536E-2</v>
       </c>
       <c r="E8" t="str">
@@ -4039,7 +4039,7 @@
         <v>106</v>
       </c>
       <c r="D9" s="33">
-        <f>B9/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>6.4220183486238536E-2</v>
       </c>
       <c r="E9" t="str">
@@ -4058,7 +4058,7 @@
         <v>105</v>
       </c>
       <c r="D10" s="33">
-        <f>B10/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>6.4220183486238536E-2</v>
       </c>
       <c r="E10" t="s">
@@ -4076,7 +4076,7 @@
         <v>103</v>
       </c>
       <c r="D11" s="33">
-        <f>B11/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>2.7522935779816515E-2</v>
       </c>
       <c r="E11" t="s">
@@ -4094,7 +4094,7 @@
         <v>125</v>
       </c>
       <c r="D12" s="33">
-        <f>B12/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>0.13761467889908258</v>
       </c>
       <c r="E12" t="s">
@@ -4112,7 +4112,7 @@
         <v>101</v>
       </c>
       <c r="D13" s="33">
-        <f>B13/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>0.11009174311926606</v>
       </c>
       <c r="E13" t="s">
@@ -4130,7 +4130,7 @@
         <v>99</v>
       </c>
       <c r="D14" s="33">
-        <f>B14/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>1.834862385321101E-2</v>
       </c>
       <c r="E14" t="str">
@@ -4149,7 +4149,7 @@
         <v>99</v>
       </c>
       <c r="D15" s="33">
-        <f>B15/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>1.834862385321101E-2</v>
       </c>
       <c r="E15" t="str">
@@ -4168,7 +4168,7 @@
         <v>99</v>
       </c>
       <c r="D16" s="33">
-        <f>B16/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>1.834862385321101E-2</v>
       </c>
       <c r="E16" t="str">
@@ -4187,7 +4187,7 @@
         <v>99</v>
       </c>
       <c r="D17" s="33">
-        <f>B17/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>1.834862385321101E-2</v>
       </c>
       <c r="E17" t="str">
@@ -4206,7 +4206,7 @@
         <v>99</v>
       </c>
       <c r="D18" s="33">
-        <f>B18/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>1.834862385321101E-2</v>
       </c>
       <c r="E18" t="str">
@@ -4225,7 +4225,7 @@
         <v>99</v>
       </c>
       <c r="D19" s="33">
-        <f>B19/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>1.834862385321101E-2</v>
       </c>
       <c r="E19" t="str">
@@ -4245,7 +4245,7 @@
         <v>98</v>
       </c>
       <c r="D20" s="33">
-        <f>B20/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>9.1743119266055051E-3</v>
       </c>
       <c r="E20" t="str">
@@ -4264,7 +4264,7 @@
         <v>98</v>
       </c>
       <c r="D21" s="33">
-        <f>B21/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>9.1743119266055051E-3</v>
       </c>
       <c r="E21" t="str">
@@ -4283,7 +4283,7 @@
         <v>98</v>
       </c>
       <c r="D22" s="33">
-        <f>B22/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>9.1743119266055051E-3</v>
       </c>
       <c r="E22" t="str">
@@ -4302,7 +4302,7 @@
         <v>98</v>
       </c>
       <c r="D23" s="33">
-        <f>B23/SUM(B:B)</f>
+        <f t="shared" si="0"/>
         <v>9.1743119266055051E-3</v>
       </c>
       <c r="E23" t="str">
@@ -4408,19 +4408,19 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f>B2+G$2*$K$2</f>
+        <f t="shared" ref="B3:B26" si="0">B2+G$2*$K$2</f>
         <v>18</v>
       </c>
       <c r="C3">
-        <f>C2+H$2*$K$2</f>
+        <f t="shared" ref="C3:C26" si="1">C2+H$2*$K$2</f>
         <v>54</v>
       </c>
       <c r="D3">
-        <f>D2+I$2*$K$2</f>
+        <f t="shared" ref="D3:D26" si="2">D2+I$2*$K$2</f>
         <v>36</v>
       </c>
       <c r="E3">
-        <f>E2+J$2*$K$2</f>
+        <f t="shared" ref="E3:E26" si="3">E2+J$2*$K$2</f>
         <v>22.5</v>
       </c>
       <c r="F3">
@@ -4439,23 +4439,23 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <f>B3+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="C4">
-        <f>C3+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>108</v>
       </c>
       <c r="D4">
-        <f>D3+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="E4">
-        <f>E3+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F7" si="0">F3+$K$2*$J$2</f>
+        <f t="shared" ref="F4:F7" si="4">F3+$K$2*$J$2</f>
         <v>45</v>
       </c>
       <c r="G4">
@@ -4467,23 +4467,23 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f>B4+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="C5">
-        <f>C4+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="D5">
-        <f>D4+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>108</v>
       </c>
       <c r="E5">
-        <f>E4+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>67.5</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>67.5</v>
       </c>
       <c r="G5">
@@ -4495,23 +4495,23 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <f>B5+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="C6">
-        <f>C5+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>216</v>
       </c>
       <c r="D6">
-        <f>D5+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="E6">
-        <f>E5+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="G6">
@@ -4523,23 +4523,23 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <f>B6+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="C7">
-        <f>C6+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>270</v>
       </c>
       <c r="D7">
-        <f>D6+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="E7">
-        <f>E6+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>112.5</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>112.5</v>
       </c>
       <c r="G7">
@@ -4554,19 +4554,19 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <f>B7+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="C8">
-        <f>C7+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>324</v>
       </c>
       <c r="D8">
-        <f>D7+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E8">
-        <f>E7+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>135</v>
       </c>
       <c r="F8">
@@ -4585,23 +4585,23 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <f>B8+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>126</v>
       </c>
       <c r="C9">
-        <f>C8+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>378</v>
       </c>
       <c r="D9">
-        <f>D8+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>252</v>
       </c>
       <c r="E9">
-        <f>E8+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>157.5</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:F26" si="1">F8+15*0.5+2*6*G9*$K$2</f>
+        <f t="shared" ref="F9:F26" si="5">F8+15*0.5+2*6*G9*$K$2</f>
         <v>343.5</v>
       </c>
       <c r="G9">
@@ -4616,23 +4616,23 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <f>B9+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="C10">
-        <f>C9+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>432</v>
       </c>
       <c r="D10">
-        <f>D9+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>288</v>
       </c>
       <c r="E10">
-        <f>E9+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>459</v>
       </c>
       <c r="G10">
@@ -4647,23 +4647,23 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <f>B10+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>162</v>
       </c>
       <c r="C11">
-        <f>C10+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>486</v>
       </c>
       <c r="D11">
-        <f>D10+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>324</v>
       </c>
       <c r="E11">
-        <f>E10+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>202.5</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>574.5</v>
       </c>
       <c r="G11">
@@ -4678,23 +4678,23 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <f>B11+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="C12">
-        <f>C11+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>540</v>
       </c>
       <c r="D12">
-        <f>D11+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>360</v>
       </c>
       <c r="E12">
-        <f>E11+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>225</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>690</v>
       </c>
       <c r="G12">
@@ -4709,23 +4709,23 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <f>B12+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>198</v>
       </c>
       <c r="C13">
-        <f>C12+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>594</v>
       </c>
       <c r="D13">
-        <f>D12+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>396</v>
       </c>
       <c r="E13">
-        <f>E12+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>247.5</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>805.5</v>
       </c>
       <c r="G13">
@@ -4740,23 +4740,23 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <f>B13+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>216</v>
       </c>
       <c r="C14">
-        <f>C13+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>648</v>
       </c>
       <c r="D14">
-        <f>D13+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>432</v>
       </c>
       <c r="E14">
-        <f>E13+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>270</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>921</v>
       </c>
       <c r="G14">
@@ -4768,23 +4768,23 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <f>B14+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>234</v>
       </c>
       <c r="C15">
-        <f>C14+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>702</v>
       </c>
       <c r="D15">
-        <f>D14+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>468</v>
       </c>
       <c r="E15">
-        <f>E14+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>292.5</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1036.5</v>
       </c>
       <c r="G15">
@@ -4796,23 +4796,23 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <f>B15+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>252</v>
       </c>
       <c r="C16">
-        <f>C15+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>756</v>
       </c>
       <c r="D16">
-        <f>D15+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>504</v>
       </c>
       <c r="E16">
-        <f>E15+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>315</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1152</v>
       </c>
       <c r="G16">
@@ -4824,23 +4824,23 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <f>B16+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>270</v>
       </c>
       <c r="C17">
-        <f>C16+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>810</v>
       </c>
       <c r="D17">
-        <f>D16+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
       <c r="E17">
-        <f>E16+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>337.5</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1267.5</v>
       </c>
       <c r="G17">
@@ -4852,23 +4852,23 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <f>B17+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>288</v>
       </c>
       <c r="C18">
-        <f>C17+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>864</v>
       </c>
       <c r="D18">
-        <f>D17+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>576</v>
       </c>
       <c r="E18">
-        <f>E17+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>360</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1383</v>
       </c>
       <c r="G18">
@@ -4880,23 +4880,23 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <f>B18+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>306</v>
       </c>
       <c r="C19">
-        <f>C18+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>918</v>
       </c>
       <c r="D19">
-        <f>D18+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>612</v>
       </c>
       <c r="E19">
-        <f>E18+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>382.5</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1498.5</v>
       </c>
       <c r="G19">
@@ -4908,23 +4908,23 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <f>B19+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>324</v>
       </c>
       <c r="C20">
-        <f>C19+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>972</v>
       </c>
       <c r="D20">
-        <f>D19+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>648</v>
       </c>
       <c r="E20">
-        <f>E19+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>405</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1614</v>
       </c>
       <c r="G20">
@@ -4936,23 +4936,23 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <f>B20+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>342</v>
       </c>
       <c r="C21">
-        <f>C20+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>1026</v>
       </c>
       <c r="D21">
-        <f>D20+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>684</v>
       </c>
       <c r="E21">
-        <f>E20+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>427.5</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1729.5</v>
       </c>
       <c r="G21">
@@ -4964,23 +4964,23 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <f>B21+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>360</v>
       </c>
       <c r="C22">
-        <f>C21+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>1080</v>
       </c>
       <c r="D22">
-        <f>D21+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>720</v>
       </c>
       <c r="E22">
-        <f>E21+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>450</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1845</v>
       </c>
       <c r="G22">
@@ -4992,23 +4992,23 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <f>B22+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>378</v>
       </c>
       <c r="C23">
-        <f>C22+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>1134</v>
       </c>
       <c r="D23">
-        <f>D22+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>756</v>
       </c>
       <c r="E23">
-        <f>E22+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>472.5</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1960.5</v>
       </c>
       <c r="G23">
@@ -5020,23 +5020,23 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <f>B23+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>396</v>
       </c>
       <c r="C24">
-        <f>C23+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>1188</v>
       </c>
       <c r="D24">
-        <f>D23+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>792</v>
       </c>
       <c r="E24">
-        <f>E23+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>495</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2076</v>
       </c>
       <c r="G24">
@@ -5048,23 +5048,23 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <f>B24+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>414</v>
       </c>
       <c r="C25">
-        <f>C24+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>1242</v>
       </c>
       <c r="D25">
-        <f>D24+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>828</v>
       </c>
       <c r="E25">
-        <f>E24+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>517.5</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2191.5</v>
       </c>
       <c r="G25">
@@ -5076,23 +5076,23 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <f>B25+G$2*$K$2</f>
+        <f t="shared" si="0"/>
         <v>432</v>
       </c>
       <c r="C26">
-        <f>C25+H$2*$K$2</f>
+        <f t="shared" si="1"/>
         <v>1296</v>
       </c>
       <c r="D26">
-        <f>D25+I$2*$K$2</f>
+        <f t="shared" si="2"/>
         <v>864</v>
       </c>
       <c r="E26">
-        <f>E25+J$2*$K$2</f>
+        <f t="shared" si="3"/>
         <v>540</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2307</v>
       </c>
       <c r="G26">

</xml_diff>